<commit_message>
Replace outdated image files with updated PNG versions for temperature, humidity, nutrient fluid temperature, TDS, and pH; add new preprocessing and evaluation visuals.
</commit_message>
<xml_diff>
--- a/Post/Index/Lampiran/Akusisi Data/sample_data.xlsx
+++ b/Post/Index/Lampiran/Akusisi Data/sample_data.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,428 +457,218 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>maxTds</t>
+          <t>waterTemperature</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>minTds</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>ph</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>tds</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>waterTemperature</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>fertilizer</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>fertilizerPumpStatus</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>nutrient</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>nutrientPumpStatus</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45599.49375</v>
+        <v>45598.04027777778</v>
       </c>
       <c r="B2" t="n">
-        <v>27.29</v>
+        <v>29.39999999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>84.00857142857141</v>
       </c>
       <c r="D2" t="n">
-        <v>1000</v>
+        <v>26.69000000000002</v>
       </c>
       <c r="E2" t="n">
-        <v>800</v>
+        <v>6.360857142857142</v>
       </c>
       <c r="F2" t="n">
-        <v>6.39</v>
-      </c>
-      <c r="G2" t="n">
-        <v>837</v>
-      </c>
-      <c r="H2" t="n">
-        <v>27.69</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
+        <v>882.8571428571429</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45600.22916666666</v>
+        <v>45598.17222222222</v>
       </c>
       <c r="B3" t="n">
-        <v>27.93</v>
+        <v>33.08857142857143</v>
       </c>
       <c r="C3" t="n">
-        <v>96.44</v>
+        <v>68.68333333333338</v>
       </c>
       <c r="D3" t="n">
-        <v>1000</v>
+        <v>26.88</v>
       </c>
       <c r="E3" t="n">
-        <v>800</v>
+        <v>6.413888888888888</v>
       </c>
       <c r="F3" t="n">
-        <v>6.43</v>
-      </c>
-      <c r="G3" t="n">
-        <v>924</v>
-      </c>
-      <c r="H3" t="n">
-        <v>27.94</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
+        <v>876.4444444444445</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45600.65</v>
+        <v>45609.45486111111</v>
       </c>
       <c r="B4" t="n">
-        <v>24.8</v>
+        <v>29.5</v>
       </c>
       <c r="C4" t="n">
-        <v>100</v>
+        <v>84.67428571428574</v>
       </c>
       <c r="D4" t="n">
-        <v>1000</v>
+        <v>28.5</v>
       </c>
       <c r="E4" t="n">
-        <v>800</v>
+        <v>6.286857142857143</v>
       </c>
       <c r="F4" t="n">
-        <v>6.34</v>
-      </c>
-      <c r="G4" t="n">
-        <v>959</v>
-      </c>
-      <c r="H4" t="n">
-        <v>26.39</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
+        <v>899.5428571428571</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45608.23888888889</v>
+        <v>45613.02777777778</v>
       </c>
       <c r="B5" t="n">
-        <v>30.3</v>
+        <v>29.79969135802468</v>
       </c>
       <c r="C5" t="n">
-        <v>80.39</v>
+        <v>84.94857142857146</v>
       </c>
       <c r="D5" t="n">
-        <v>1000</v>
+        <v>26.99828571428572</v>
       </c>
       <c r="E5" t="n">
-        <v>800</v>
+        <v>6.322571428571426</v>
       </c>
       <c r="F5" t="n">
-        <v>6.41</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1249</v>
-      </c>
-      <c r="H5" t="n">
-        <v>27.94</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
+        <v>812.2857142857143</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45611.42708333334</v>
+        <v>45621.03958333333</v>
       </c>
       <c r="B6" t="n">
-        <v>27.8</v>
+        <v>29.41388888888888</v>
       </c>
       <c r="C6" t="n">
-        <v>97.31</v>
+        <v>85.75833333333334</v>
       </c>
       <c r="D6" t="n">
-        <v>1000</v>
+        <v>27.05999999999997</v>
       </c>
       <c r="E6" t="n">
-        <v>800</v>
+        <v>6.335277777777778</v>
       </c>
       <c r="F6" t="n">
-        <v>6.31</v>
-      </c>
-      <c r="G6" t="n">
-        <v>833</v>
-      </c>
-      <c r="H6" t="n">
-        <v>27.55</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
+        <v>750.9166666666666</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45611.49236111111</v>
+        <v>45622.27013888889</v>
       </c>
       <c r="B7" t="n">
-        <v>27.4</v>
+        <v>32.05428571428572</v>
       </c>
       <c r="C7" t="n">
-        <v>96.42</v>
+        <v>77.72571428571429</v>
       </c>
       <c r="D7" t="n">
-        <v>1000</v>
+        <v>27.25</v>
       </c>
       <c r="E7" t="n">
-        <v>800</v>
+        <v>6.353714285714286</v>
       </c>
       <c r="F7" t="n">
-        <v>6.28</v>
-      </c>
-      <c r="G7" t="n">
-        <v>831</v>
-      </c>
-      <c r="H7" t="n">
-        <v>27.56</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
+        <v>735.8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45611.85694444444</v>
+        <v>45624.02777777778</v>
       </c>
       <c r="B8" t="n">
-        <v>26.2</v>
+        <v>29.8742857142857</v>
       </c>
       <c r="C8" t="n">
-        <v>100</v>
+        <v>88.32000000000004</v>
       </c>
       <c r="D8" t="n">
-        <v>1000</v>
+        <v>26.79114285714284</v>
       </c>
       <c r="E8" t="n">
-        <v>800</v>
+        <v>6.321714285714286</v>
       </c>
       <c r="F8" t="n">
-        <v>6.29</v>
-      </c>
-      <c r="G8" t="n">
-        <v>817</v>
-      </c>
-      <c r="H8" t="n">
-        <v>27.15</v>
-      </c>
-      <c r="I8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" t="n">
-        <v>1</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
+        <v>743.3428571428572</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45624.49722222222</v>
+        <v>45625.65902777778</v>
       </c>
       <c r="B9" t="n">
-        <v>28.02</v>
+        <v>27</v>
       </c>
       <c r="C9" t="n">
-        <v>95.52</v>
+        <v>97.89444444444452</v>
       </c>
       <c r="D9" t="n">
-        <v>1000</v>
+        <v>27.38</v>
       </c>
       <c r="E9" t="n">
-        <v>800</v>
+        <v>6.320277777777776</v>
       </c>
       <c r="F9" t="n">
-        <v>6.34</v>
-      </c>
-      <c r="G9" t="n">
-        <v>772</v>
-      </c>
-      <c r="H9" t="n">
-        <v>27.49</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0</v>
+        <v>775.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45624.68472222222</v>
+        <v>45627.125</v>
       </c>
       <c r="B10" t="n">
-        <v>25.71</v>
+        <v>26.95428571428571</v>
       </c>
       <c r="C10" t="n">
-        <v>100</v>
+        <v>97.92857142857146</v>
       </c>
       <c r="D10" t="n">
-        <v>1000</v>
+        <v>26.44000000000002</v>
       </c>
       <c r="E10" t="n">
-        <v>800</v>
+        <v>6.239428571428573</v>
       </c>
       <c r="F10" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="G10" t="n">
-        <v>763</v>
-      </c>
-      <c r="H10" t="n">
-        <v>27.28</v>
-      </c>
-      <c r="I10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
+        <v>987.5714285714286</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45627.64861111111</v>
+        <v>45627.64444444444</v>
       </c>
       <c r="B11" t="n">
-        <v>25.87</v>
+        <v>25.82857142857141</v>
       </c>
       <c r="C11" t="n">
         <v>100</v>
       </c>
       <c r="D11" t="n">
-        <v>1000</v>
+        <v>26.54742857142855</v>
       </c>
       <c r="E11" t="n">
-        <v>800</v>
+        <v>6.259428571428571</v>
       </c>
       <c r="F11" t="n">
-        <v>6.26</v>
-      </c>
-      <c r="G11" t="n">
-        <v>876</v>
-      </c>
-      <c r="H11" t="n">
-        <v>26.61</v>
-      </c>
-      <c r="I11" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" t="n">
-        <v>1</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0</v>
+        <v>975.3714285714286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>